<commit_message>
Sprint 8 - In Progress
</commit_message>
<xml_diff>
--- a/WSI-PageLoadPerformance.xlsx
+++ b/WSI-PageLoadPerformance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18600" windowHeight="6840" firstSheet="4" activeTab="7"/>
+    <workbookView windowWidth="18600" windowHeight="6840" firstSheet="10" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,19 @@
     <sheet name="25Jun2020 22.50.02" sheetId="6" r:id="rId6"/>
     <sheet name="26Jun2020 14.42.21" sheetId="7" r:id="rId7"/>
     <sheet name="26Jun2020 14.46.40" sheetId="8" r:id="rId8"/>
+    <sheet name="29Jun2020 12.41.12" sheetId="9" r:id="rId9"/>
+    <sheet name="29Jun2020 13.36.14" sheetId="10" r:id="rId10"/>
+    <sheet name="30Jun2020 12.31.21" sheetId="11" r:id="rId11"/>
+    <sheet name="30Jun2020 14.07.40" sheetId="12" r:id="rId12"/>
+    <sheet name="30Jun2020 15.58.03" sheetId="13" r:id="rId13"/>
+    <sheet name="30Jun2020 16.13.28" sheetId="14" r:id="rId14"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="47">
   <si>
     <t>Test</t>
   </si>
@@ -154,6 +160,15 @@
   <si>
     <t>User &amp; Role Management Roles</t>
   </si>
+  <si>
+    <t>User &amp; Role Management &gt; Users</t>
+  </si>
+  <si>
+    <t>User &amp; Role Management &gt; Roles</t>
+  </si>
+  <si>
+    <t>User &amp; Role Management &gt; Permissions</t>
+  </si>
 </sst>
 </file>
 
@@ -161,9 +176,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -174,48 +189,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -244,14 +220,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -267,7 +235,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -280,9 +248,55 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -303,8 +317,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -327,115 +342,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -465,7 +378,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -477,19 +486,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -540,6 +555,39 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
@@ -556,30 +604,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -609,24 +633,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -635,136 +653,133 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1110,6 +1125,2294 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C78"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1078</v>
+      </c>
+      <c r="C2">
+        <v>10210</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>631</v>
+      </c>
+      <c r="C3">
+        <v>3644</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>1120</v>
+      </c>
+      <c r="C4">
+        <v>9655</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5">
+        <v>775</v>
+      </c>
+      <c r="C5">
+        <v>4658</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1049</v>
+      </c>
+      <c r="C6">
+        <v>7405</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1282</v>
+      </c>
+      <c r="C7">
+        <v>8154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>796</v>
+      </c>
+      <c r="C8">
+        <v>8624</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>986</v>
+      </c>
+      <c r="C9">
+        <v>3730</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>1068</v>
+      </c>
+      <c r="C10">
+        <v>8656</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>1153</v>
+      </c>
+      <c r="C11">
+        <v>5237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>1459</v>
+      </c>
+      <c r="C12">
+        <v>8740</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>1028</v>
+      </c>
+      <c r="C13">
+        <v>14969</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1732</v>
+      </c>
+      <c r="C14">
+        <v>8200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>779</v>
+      </c>
+      <c r="C15">
+        <v>2780</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>1384</v>
+      </c>
+      <c r="C16">
+        <v>8210</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17">
+        <v>870</v>
+      </c>
+      <c r="C17">
+        <v>6020</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>1281</v>
+      </c>
+      <c r="C18">
+        <v>7823</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>1513</v>
+      </c>
+      <c r="C19">
+        <v>4704</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>1821</v>
+      </c>
+      <c r="C20">
+        <v>9762</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>691</v>
+      </c>
+      <c r="C21">
+        <v>3413</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>1585</v>
+      </c>
+      <c r="C22">
+        <v>9539</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>1043</v>
+      </c>
+      <c r="C23">
+        <v>4475</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>734</v>
+      </c>
+      <c r="C24">
+        <v>10753</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>936</v>
+      </c>
+      <c r="C25">
+        <v>4131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>1014</v>
+      </c>
+      <c r="C26">
+        <v>7926</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>599</v>
+      </c>
+      <c r="C27">
+        <v>4161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>1099</v>
+      </c>
+      <c r="C28">
+        <v>8698</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29">
+        <v>614</v>
+      </c>
+      <c r="C29">
+        <v>3671</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>1084</v>
+      </c>
+      <c r="C30">
+        <v>9300</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>871</v>
+      </c>
+      <c r="C31">
+        <v>3027</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <v>1101</v>
+      </c>
+      <c r="C32">
+        <v>8513</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33">
+        <v>1029</v>
+      </c>
+      <c r="C33">
+        <v>5058</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <v>1085</v>
+      </c>
+      <c r="C34">
+        <v>9176</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>603</v>
+      </c>
+      <c r="C35">
+        <v>15996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <v>2484</v>
+      </c>
+      <c r="C36">
+        <v>12684</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37">
+        <v>1137</v>
+      </c>
+      <c r="C37">
+        <v>26956</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>5201</v>
+      </c>
+      <c r="C38">
+        <v>17457</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39">
+        <v>639</v>
+      </c>
+      <c r="C39">
+        <v>3146</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>1179</v>
+      </c>
+      <c r="C40">
+        <v>8653</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <v>1069</v>
+      </c>
+      <c r="C41">
+        <v>8095</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42">
+        <v>640</v>
+      </c>
+      <c r="C42">
+        <v>6812</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43">
+        <v>1311</v>
+      </c>
+      <c r="C43">
+        <v>8976</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>23</v>
+      </c>
+      <c r="B44">
+        <v>1063</v>
+      </c>
+      <c r="C44">
+        <v>3952</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>4</v>
+      </c>
+      <c r="B45">
+        <v>882</v>
+      </c>
+      <c r="C45">
+        <v>8715</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46">
+        <v>662</v>
+      </c>
+      <c r="C46">
+        <v>4102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>4</v>
+      </c>
+      <c r="B47">
+        <v>1151</v>
+      </c>
+      <c r="C47">
+        <v>10534</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>25</v>
+      </c>
+      <c r="B48">
+        <v>900</v>
+      </c>
+      <c r="C48">
+        <v>6042</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49">
+        <v>1034</v>
+      </c>
+      <c r="C49">
+        <v>11407</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50">
+        <v>646</v>
+      </c>
+      <c r="C50">
+        <v>3530</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51">
+        <v>1122</v>
+      </c>
+      <c r="C51">
+        <v>8368</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52">
+        <v>739</v>
+      </c>
+      <c r="C52">
+        <v>4274</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>4</v>
+      </c>
+      <c r="B53">
+        <v>1539</v>
+      </c>
+      <c r="C53">
+        <v>12232</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54">
+        <v>722</v>
+      </c>
+      <c r="C54">
+        <v>3726</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>4</v>
+      </c>
+      <c r="B55">
+        <v>1067</v>
+      </c>
+      <c r="C55">
+        <v>8467</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56">
+        <v>1297</v>
+      </c>
+      <c r="C56">
+        <v>5738</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>4</v>
+      </c>
+      <c r="B57">
+        <v>1240</v>
+      </c>
+      <c r="C57">
+        <v>8615</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58">
+        <v>642</v>
+      </c>
+      <c r="C58">
+        <v>3792</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>4</v>
+      </c>
+      <c r="B59">
+        <v>887</v>
+      </c>
+      <c r="C59">
+        <v>11040</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60">
+        <v>1599</v>
+      </c>
+      <c r="C60">
+        <v>5424</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>4</v>
+      </c>
+      <c r="B61">
+        <v>5038</v>
+      </c>
+      <c r="C61">
+        <v>11893</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>41</v>
+      </c>
+      <c r="B62">
+        <v>930</v>
+      </c>
+      <c r="C62">
+        <v>6227</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63">
+        <v>1131</v>
+      </c>
+      <c r="C63">
+        <v>7115</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>31</v>
+      </c>
+      <c r="B64">
+        <v>788</v>
+      </c>
+      <c r="C64">
+        <v>4399</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65">
+        <v>1329</v>
+      </c>
+      <c r="C65">
+        <v>10764</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>42</v>
+      </c>
+      <c r="B66">
+        <v>605</v>
+      </c>
+      <c r="C66">
+        <v>3592</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>4</v>
+      </c>
+      <c r="B67">
+        <v>853</v>
+      </c>
+      <c r="C67">
+        <v>10513</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>32</v>
+      </c>
+      <c r="B68">
+        <v>756</v>
+      </c>
+      <c r="C68">
+        <v>7348</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>4</v>
+      </c>
+      <c r="B69">
+        <v>786</v>
+      </c>
+      <c r="C69">
+        <v>7533</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>33</v>
+      </c>
+      <c r="B70">
+        <v>761</v>
+      </c>
+      <c r="C70">
+        <v>6065</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71">
+        <v>1263</v>
+      </c>
+      <c r="C71">
+        <v>8895</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>34</v>
+      </c>
+      <c r="B72">
+        <v>901</v>
+      </c>
+      <c r="C72">
+        <v>13208</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73">
+        <v>1068</v>
+      </c>
+      <c r="C73">
+        <v>12992</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>43</v>
+      </c>
+      <c r="B74">
+        <v>710</v>
+      </c>
+      <c r="C74">
+        <v>3712</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75">
+        <v>1712</v>
+      </c>
+      <c r="C75">
+        <v>9823</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>35</v>
+      </c>
+      <c r="B76">
+        <v>881</v>
+      </c>
+      <c r="C76">
+        <v>22994</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>4</v>
+      </c>
+      <c r="B77">
+        <v>2260</v>
+      </c>
+      <c r="C77">
+        <v>10119</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>36</v>
+      </c>
+      <c r="B78">
+        <v>625</v>
+      </c>
+      <c r="C78">
+        <v>1592</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1491</v>
+      </c>
+      <c r="C2">
+        <v>10732</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>882</v>
+      </c>
+      <c r="C3">
+        <v>11075</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>925</v>
+      </c>
+      <c r="C4">
+        <v>6975</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1551</v>
+      </c>
+      <c r="C5">
+        <v>7385</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1242</v>
+      </c>
+      <c r="C2">
+        <v>10940</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>759</v>
+      </c>
+      <c r="C3">
+        <v>3773</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>985</v>
+      </c>
+      <c r="C4">
+        <v>11240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5">
+        <v>1277</v>
+      </c>
+      <c r="C5">
+        <v>4924</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1209</v>
+      </c>
+      <c r="C6">
+        <v>14767</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>619</v>
+      </c>
+      <c r="C7">
+        <v>6913</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>727</v>
+      </c>
+      <c r="C8">
+        <v>7012</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>757</v>
+      </c>
+      <c r="C9">
+        <v>3268</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>1149</v>
+      </c>
+      <c r="C10">
+        <v>7626</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>834</v>
+      </c>
+      <c r="C11">
+        <v>3680</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>2096</v>
+      </c>
+      <c r="C12">
+        <v>17686</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>651</v>
+      </c>
+      <c r="C13">
+        <v>9154</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>3601</v>
+      </c>
+      <c r="C14">
+        <v>13901</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>692</v>
+      </c>
+      <c r="C15">
+        <v>2874</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>1094</v>
+      </c>
+      <c r="C16">
+        <v>16523</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17">
+        <v>760</v>
+      </c>
+      <c r="C17">
+        <v>5439</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>1113</v>
+      </c>
+      <c r="C18">
+        <v>12496</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>785</v>
+      </c>
+      <c r="C19">
+        <v>2997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>1116</v>
+      </c>
+      <c r="C20">
+        <v>12894</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>904</v>
+      </c>
+      <c r="C21">
+        <v>4396</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>1191</v>
+      </c>
+      <c r="C22">
+        <v>20621</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>713</v>
+      </c>
+      <c r="C23">
+        <v>4213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>1078</v>
+      </c>
+      <c r="C24">
+        <v>9598</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>751</v>
+      </c>
+      <c r="C25">
+        <v>3758</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>1163</v>
+      </c>
+      <c r="C26">
+        <v>8739</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27">
+        <v>1218</v>
+      </c>
+      <c r="C27">
+        <v>4152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>1057</v>
+      </c>
+      <c r="C28">
+        <v>8947</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29">
+        <v>1276</v>
+      </c>
+      <c r="C29">
+        <v>4355</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>1172</v>
+      </c>
+      <c r="C30">
+        <v>13944</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31">
+        <v>796</v>
+      </c>
+      <c r="C31">
+        <v>3808</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <v>1089</v>
+      </c>
+      <c r="C32">
+        <v>8698</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33">
+        <v>692</v>
+      </c>
+      <c r="C33">
+        <v>4819</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <v>1126</v>
+      </c>
+      <c r="C34">
+        <v>9904</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>634</v>
+      </c>
+      <c r="C35">
+        <v>7738</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <v>700</v>
+      </c>
+      <c r="C36">
+        <v>7221</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37">
+        <v>1197</v>
+      </c>
+      <c r="C37">
+        <v>8974</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>798</v>
+      </c>
+      <c r="C38">
+        <v>15484</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39">
+        <v>1159</v>
+      </c>
+      <c r="C39">
+        <v>4409</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>1080</v>
+      </c>
+      <c r="C40">
+        <v>12494</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>21</v>
+      </c>
+      <c r="B41">
+        <v>738</v>
+      </c>
+      <c r="C41">
+        <v>4663</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>1653</v>
+      </c>
+      <c r="C42">
+        <v>10425</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43">
+        <v>994</v>
+      </c>
+      <c r="C43">
+        <v>11011</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44">
+        <v>1124</v>
+      </c>
+      <c r="C44">
+        <v>9835</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45">
+        <v>693</v>
+      </c>
+      <c r="C45">
+        <v>4102</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>4</v>
+      </c>
+      <c r="B46">
+        <v>1164</v>
+      </c>
+      <c r="C46">
+        <v>7708</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47">
+        <v>847</v>
+      </c>
+      <c r="C47">
+        <v>4510</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48">
+        <v>1078</v>
+      </c>
+      <c r="C48">
+        <v>14894</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49">
+        <v>674</v>
+      </c>
+      <c r="C49">
+        <v>9466</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>4</v>
+      </c>
+      <c r="B50">
+        <v>1381</v>
+      </c>
+      <c r="C50">
+        <v>8828</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3">
+      <c r="A51" t="s">
+        <v>26</v>
+      </c>
+      <c r="B51">
+        <v>913</v>
+      </c>
+      <c r="C51">
+        <v>3973</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <v>1056</v>
+      </c>
+      <c r="C52">
+        <v>8835</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>37</v>
+      </c>
+      <c r="B53">
+        <v>876</v>
+      </c>
+      <c r="C53">
+        <v>4330</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54">
+        <v>1089</v>
+      </c>
+      <c r="C54">
+        <v>9523</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55">
+        <v>855</v>
+      </c>
+      <c r="C55">
+        <v>4191</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56">
+        <v>1328</v>
+      </c>
+      <c r="C56">
+        <v>8594</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>28</v>
+      </c>
+      <c r="B57">
+        <v>1794</v>
+      </c>
+      <c r="C57">
+        <v>5114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>4</v>
+      </c>
+      <c r="B58">
+        <v>1063</v>
+      </c>
+      <c r="C58">
+        <v>12320</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59">
+        <v>901</v>
+      </c>
+      <c r="C59">
+        <v>5906</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>4</v>
+      </c>
+      <c r="B60">
+        <v>1138</v>
+      </c>
+      <c r="C60">
+        <v>7905</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
+        <v>30</v>
+      </c>
+      <c r="B61">
+        <v>979</v>
+      </c>
+      <c r="C61">
+        <v>4241</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>4</v>
+      </c>
+      <c r="B62">
+        <v>779</v>
+      </c>
+      <c r="C62">
+        <v>7693</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B63">
+        <v>873</v>
+      </c>
+      <c r="C63">
+        <v>8111</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>4</v>
+      </c>
+      <c r="B64">
+        <v>772</v>
+      </c>
+      <c r="C64">
+        <v>13749</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65">
+        <v>901</v>
+      </c>
+      <c r="C65">
+        <v>4301</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>4</v>
+      </c>
+      <c r="B66">
+        <v>1041</v>
+      </c>
+      <c r="C66">
+        <v>8487</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>32</v>
+      </c>
+      <c r="B67">
+        <v>648</v>
+      </c>
+      <c r="C67">
+        <v>5019</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>4</v>
+      </c>
+      <c r="B68">
+        <v>1303</v>
+      </c>
+      <c r="C68">
+        <v>10911</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>33</v>
+      </c>
+      <c r="B69">
+        <v>867</v>
+      </c>
+      <c r="C69">
+        <v>7172</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>4</v>
+      </c>
+      <c r="B70">
+        <v>1735</v>
+      </c>
+      <c r="C70">
+        <v>9681</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>34</v>
+      </c>
+      <c r="B71">
+        <v>9645</v>
+      </c>
+      <c r="C71">
+        <v>38778</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>4</v>
+      </c>
+      <c r="B72">
+        <v>1124</v>
+      </c>
+      <c r="C72">
+        <v>8495</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>4</v>
+      </c>
+      <c r="B73">
+        <v>1168</v>
+      </c>
+      <c r="C73">
+        <v>9222</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>4</v>
+      </c>
+      <c r="B74">
+        <v>1401</v>
+      </c>
+      <c r="C74">
+        <v>10675</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>44</v>
+      </c>
+      <c r="B75">
+        <v>710</v>
+      </c>
+      <c r="C75">
+        <v>404</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="65.2727272727273" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1110</v>
+      </c>
+      <c r="C2">
+        <v>8568</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>554</v>
+      </c>
+      <c r="C3">
+        <v>2835</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4">
+        <v>688</v>
+      </c>
+      <c r="C4">
+        <v>4449</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>633</v>
+      </c>
+      <c r="C5">
+        <v>7010</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>647</v>
+      </c>
+      <c r="C6">
+        <v>3036</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>767</v>
+      </c>
+      <c r="C7">
+        <v>3502</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8">
+        <v>670</v>
+      </c>
+      <c r="C8">
+        <v>8143</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>604</v>
+      </c>
+      <c r="C9">
+        <v>3030</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10">
+        <v>716</v>
+      </c>
+      <c r="C10">
+        <v>3515</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>661</v>
+      </c>
+      <c r="C11">
+        <v>3799</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>620</v>
+      </c>
+      <c r="C12">
+        <v>2873</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>806</v>
+      </c>
+      <c r="C13">
+        <v>3610</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14">
+        <v>726</v>
+      </c>
+      <c r="C14">
+        <v>4628</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15">
+        <v>1043</v>
+      </c>
+      <c r="C15">
+        <v>4659</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16">
+        <v>804</v>
+      </c>
+      <c r="C16">
+        <v>3525</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>822</v>
+      </c>
+      <c r="C17">
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>762</v>
+      </c>
+      <c r="C18">
+        <v>5014</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>1063</v>
+      </c>
+      <c r="C19">
+        <v>8637</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>1067</v>
+      </c>
+      <c r="C20">
+        <v>10970</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>776</v>
+      </c>
+      <c r="C21">
+        <v>4141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>817</v>
+      </c>
+      <c r="C22">
+        <v>4415</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>875</v>
+      </c>
+      <c r="C23">
+        <v>7035</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>1141</v>
+      </c>
+      <c r="C24">
+        <v>8033</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>679</v>
+      </c>
+      <c r="C25">
+        <v>3642</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>607</v>
+      </c>
+      <c r="C26">
+        <v>6041</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>591</v>
+      </c>
+      <c r="C27">
+        <v>4125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28">
+        <v>684</v>
+      </c>
+      <c r="C28">
+        <v>4348</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>721</v>
+      </c>
+      <c r="C29">
+        <v>3705</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>1080</v>
+      </c>
+      <c r="C30">
+        <v>8669</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>716</v>
+      </c>
+      <c r="C31">
+        <v>3978</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32">
+        <v>728</v>
+      </c>
+      <c r="C32">
+        <v>4177</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>773</v>
+      </c>
+      <c r="C33">
+        <v>5815</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>697</v>
+      </c>
+      <c r="C34">
+        <v>4255</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>999</v>
+      </c>
+      <c r="C35">
+        <v>4233</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <v>1030</v>
+      </c>
+      <c r="C36">
+        <v>5201</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37">
+        <v>1059</v>
+      </c>
+      <c r="C37">
+        <v>9002</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38">
+        <v>731</v>
+      </c>
+      <c r="C38">
+        <v>19326</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39">
+        <v>667</v>
+      </c>
+      <c r="C39">
+        <v>3924</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40">
+        <v>705</v>
+      </c>
+      <c r="C40">
+        <v>27803</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41">
+        <v>588</v>
+      </c>
+      <c r="C41">
+        <v>663</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
@@ -2174,7 +4477,7 @@
   <sheetPr/>
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -2639,4 +4942,483 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="2"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1259</v>
+      </c>
+      <c r="C2">
+        <v>9854</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>804</v>
+      </c>
+      <c r="C3">
+        <v>4194</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3976</v>
+      </c>
+      <c r="C4">
+        <v>17419</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5">
+        <v>1074</v>
+      </c>
+      <c r="C5">
+        <v>4533</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>1135</v>
+      </c>
+      <c r="C6">
+        <v>7575</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>825</v>
+      </c>
+      <c r="C7">
+        <v>8566</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>2165</v>
+      </c>
+      <c r="C8">
+        <v>12811</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1251</v>
+      </c>
+      <c r="C9">
+        <v>6450</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>1663</v>
+      </c>
+      <c r="C10">
+        <v>16948</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11">
+        <v>1167</v>
+      </c>
+      <c r="C11">
+        <v>18733</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12">
+        <v>1718</v>
+      </c>
+      <c r="C12">
+        <v>18240</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13">
+        <v>3942</v>
+      </c>
+      <c r="C13">
+        <v>12544</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1296</v>
+      </c>
+      <c r="C14">
+        <v>10605</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15">
+        <v>1223</v>
+      </c>
+      <c r="C15">
+        <v>9368</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>1373</v>
+      </c>
+      <c r="C16">
+        <v>8814</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17">
+        <v>1219</v>
+      </c>
+      <c r="C17">
+        <v>23153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>2194</v>
+      </c>
+      <c r="C18">
+        <v>12542</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>1078</v>
+      </c>
+      <c r="C19">
+        <v>8820</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20">
+        <v>3208</v>
+      </c>
+      <c r="C20">
+        <v>13504</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21">
+        <v>8415</v>
+      </c>
+      <c r="C21">
+        <v>27024</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>1677</v>
+      </c>
+      <c r="C22">
+        <v>8759</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23">
+        <v>4898</v>
+      </c>
+      <c r="C23">
+        <v>20141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24">
+        <v>1953</v>
+      </c>
+      <c r="C24">
+        <v>14526</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25">
+        <v>14538</v>
+      </c>
+      <c r="C25">
+        <v>38412</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>2408</v>
+      </c>
+      <c r="C26">
+        <v>11772</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>4572</v>
+      </c>
+      <c r="C27">
+        <v>15175</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>6622</v>
+      </c>
+      <c r="C28">
+        <v>20889</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>2128</v>
+      </c>
+      <c r="C29">
+        <v>12421</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>1221</v>
+      </c>
+      <c r="C30">
+        <v>8124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>1107</v>
+      </c>
+      <c r="C31">
+        <v>8843</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <v>5062</v>
+      </c>
+      <c r="C32">
+        <v>27463</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33">
+        <v>1826</v>
+      </c>
+      <c r="C33">
+        <v>8839</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34">
+        <v>5240</v>
+      </c>
+      <c r="C34">
+        <v>25631</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35">
+        <v>878</v>
+      </c>
+      <c r="C35">
+        <v>11708</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36">
+        <v>1265</v>
+      </c>
+      <c r="C36">
+        <v>15403</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37">
+        <v>2000</v>
+      </c>
+      <c r="C37">
+        <v>14349</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38">
+        <v>1113</v>
+      </c>
+      <c r="C38">
+        <v>16402</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39">
+        <v>704</v>
+      </c>
+      <c r="C39">
+        <v>10885</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40">
+        <v>1636</v>
+      </c>
+      <c r="C40">
+        <v>17443</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41">
+        <v>1437</v>
+      </c>
+      <c r="C41">
+        <v>13844</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42">
+        <v>1063</v>
+      </c>
+      <c r="C42">
+        <v>11229</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Manage List Single Session-Pagination Approach
</commit_message>
<xml_diff>
--- a/WSI-PageLoadPerformance.xlsx
+++ b/WSI-PageLoadPerformance.xlsx
@@ -91,13 +91,17 @@
     <sheet name="03Aug2020 23.12.33" r:id="rId85" sheetId="82"/>
     <sheet name="03Aug2020 23.14.35" r:id="rId86" sheetId="83"/>
     <sheet name="03Aug2020 23.38.21" r:id="rId87" sheetId="84"/>
+    <sheet name="04Aug2020 23.24.06" r:id="rId88" sheetId="85"/>
+    <sheet name="05Aug2020 05.43.05" r:id="rId89" sheetId="86"/>
+    <sheet name="05Aug2020 06.12.05" r:id="rId90" sheetId="87"/>
+    <sheet name="09Aug2020 16.30.28" r:id="rId91" sheetId="88"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1683" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="57">
   <si>
     <t>Test</t>
   </si>
@@ -250,6 +254,24 @@
   </si>
   <si>
     <t>https://supplychain-mcp-user-interface-qa.services.west.nonprod.wsgc.com/</t>
+  </si>
+  <si>
+    <t>User Profile</t>
+  </si>
+  <si>
+    <t>Libraries &gt; Merch List- Page 1</t>
+  </si>
+  <si>
+    <t>Libraries &gt; Merch List- Page 2</t>
+  </si>
+  <si>
+    <t>Libraries &gt; Merch List- Page 3</t>
+  </si>
+  <si>
+    <t>Libraries &gt; Merch List- Page 4</t>
+  </si>
+  <si>
+    <t>Libraries &gt; Merch List- Page 5</t>
   </si>
 </sst>
 </file>
@@ -18834,6 +18856,705 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3059.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>54246.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1096.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>12893.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="n">
+        <v>745.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>3580.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1253.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>10131.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="n">
+        <v>686.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>6077.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1079.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>8503.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" t="n">
+        <v>863.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>6603.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="n">
+        <v>840.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>8482.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="n">
+        <v>4780.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>20628.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1304.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>30796.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1229.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>11694.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="n">
+        <v>5223.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>37333.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="n">
+        <v>2737.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>11592.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" t="n">
+        <v>2200.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>44180.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1281.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>5976.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2554.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>51017.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1828.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>16645.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2517.0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>43379.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2245.0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>20001.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="n">
+        <v>7594.0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>42823.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1705.0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>15053.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" t="n">
+        <v>6245.0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>53084.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1378.0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>23072.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" t="n">
+        <v>4388.0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>43313.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="n">
+        <v>3440.0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>5293.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" t="n">
+        <v>3698.0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>33810.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2533.0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>16231.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" t="n">
+        <v>4282.0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>32499.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="n">
+        <v>6000.0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>16261.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" t="n">
+        <v>1665.0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>14196.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" t="n">
+        <v>12111.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>3535.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="n">
+        <v>1073.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>16605.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" t="n">
+        <v>668.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" t="n">
+        <v>751.0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>7404.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" t="n">
+        <v>2028.0</v>
+      </c>
+      <c r="C36" t="n">
+        <v>37823.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37" t="n">
+        <v>1743.0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>15846.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" t="n">
+        <v>2112.0</v>
+      </c>
+      <c r="C38" t="n">
+        <v>34629.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>19</v>
+      </c>
+      <c r="B39" t="n">
+        <v>2405.0</v>
+      </c>
+      <c r="C39" t="n">
+        <v>28515.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2309.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>43951.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" t="n">
+        <v>4341.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>14223.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1160.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>13399.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1160.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>642.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="n">
+        <v>741.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>12324.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="n">
+        <v>741.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>8817.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="n">
+        <v>741.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>15221.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="n">
+        <v>741.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>14338.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="n">
+        <v>741.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>22694.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="n">
+        <v>741.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>720.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="n">
+        <v>636.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>13084.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="n">
+        <v>636.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>10239.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="n">
+        <v>636.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>14596.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="n">
+        <v>636.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>14924.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="n">
+        <v>636.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>21389.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>

</xml_diff>

<commit_message>
Latest Checkin 10 Aug 2020
</commit_message>
<xml_diff>
--- a/WSI-PageLoadPerformance.xlsx
+++ b/WSI-PageLoadPerformance.xlsx
@@ -95,13 +95,15 @@
     <sheet name="05Aug2020 05.43.05" r:id="rId89" sheetId="86"/>
     <sheet name="05Aug2020 06.12.05" r:id="rId90" sheetId="87"/>
     <sheet name="09Aug2020 16.30.28" r:id="rId91" sheetId="88"/>
+    <sheet name="09Aug2020 19.22.15" r:id="rId92" sheetId="89"/>
+    <sheet name="09Aug2020 19.24.34" r:id="rId93" sheetId="90"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1752" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1773" uniqueCount="57">
   <si>
     <t>Test</t>
   </si>
@@ -19555,6 +19557,35 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
@@ -20032,4 +20063,176 @@
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1065.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9297.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1065.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>847.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" t="n">
+        <v>765.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>17097.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="n">
+        <v>765.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>13015.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="n">
+        <v>765.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>14791.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" t="n">
+        <v>765.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>12117.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" t="n">
+        <v>765.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>11507.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="n">
+        <v>765.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>607.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" t="n">
+        <v>694.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>14989.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="n">
+        <v>694.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>14970.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" t="n">
+        <v>694.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>13032.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="n">
+        <v>694.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>13764.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="n">
+        <v>694.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>14414.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Create Placeholder - performance
</commit_message>
<xml_diff>
--- a/WSI-PageLoadPerformance.xlsx
+++ b/WSI-PageLoadPerformance.xlsx
@@ -22,13 +22,65 @@
     <sheet name="04Sep2020 19.27.32" r:id="rId16" sheetId="15"/>
     <sheet name="04Sep2020 19.37.44" r:id="rId17" sheetId="16"/>
     <sheet name="04Sep2020 20.24.46" r:id="rId18" sheetId="17"/>
+    <sheet name="16Sep2020 22.03.27(IST)-" r:id="rId19" sheetId="18"/>
+    <sheet name="17Sep2020 16.39.57(IST)-" r:id="rId20" sheetId="19"/>
+    <sheet name="17Sep2020 20.10.37(IST)-" r:id="rId21" sheetId="20"/>
+    <sheet name="17Sep2020 20.43.52(IST)-LOCAL" r:id="rId22" sheetId="21"/>
+    <sheet name="17Sep2020 20.53.19(IST)-LOCAL" r:id="rId23" sheetId="22"/>
+    <sheet name="23Sep2020 19.41.07(IST)-LOCAL" r:id="rId24" sheetId="23"/>
+    <sheet name="23Sep2020 19.43.42(IST)-LOCAL" r:id="rId25" sheetId="24"/>
+    <sheet name="23Sep2020 20.07.14(IST)-LOCAL" r:id="rId26" sheetId="25"/>
+    <sheet name="23Sep2020 21.07.40(IST)-LOCAL" r:id="rId27" sheetId="26"/>
+    <sheet name="23Sep2020 21.13.07(IST)-LOCAL" r:id="rId28" sheetId="27"/>
+    <sheet name="01Oct2020 16.33.14(IST)-LOCAL" r:id="rId29" sheetId="28"/>
+    <sheet name="01Oct2020 17.16.15(IST)-LOCAL" r:id="rId30" sheetId="29"/>
+    <sheet name="01Oct2020 17.28.42(IST)-LOCAL" r:id="rId31" sheetId="30"/>
+    <sheet name="01Oct2020 17.38.55(IST)-LOCAL" r:id="rId32" sheetId="31"/>
+    <sheet name="01Oct2020 17.50.59(IST)-LOCAL" r:id="rId33" sheetId="32"/>
+    <sheet name="13Oct2020 20.04.47(IST)-LOCAL" r:id="rId34" sheetId="33"/>
+    <sheet name="13Oct2020 20.20.54(IST)-LOCAL" r:id="rId35" sheetId="34"/>
+    <sheet name="13Oct2020 21.20.09(IST)-LOCAL" r:id="rId36" sheetId="35"/>
+    <sheet name="14Oct2020 21.52.35(IST)-LOCAL" r:id="rId37" sheetId="36"/>
+    <sheet name="02Nov2020 15.09.22(IST)-LOCAL" r:id="rId38" sheetId="37"/>
+    <sheet name="02Nov2020 15.10.40(IST)-LOCAL" r:id="rId39" sheetId="38"/>
+    <sheet name="02Nov2020 15.12.22(IST)-LOCAL" r:id="rId40" sheetId="39"/>
+    <sheet name="02Nov2020 15.13.51(IST)-LOCAL" r:id="rId41" sheetId="40"/>
+    <sheet name="02Nov2020 15.17.55(IST)-LOCAL" r:id="rId42" sheetId="41"/>
+    <sheet name="02Nov2020 15.22.22(IST)-LOCAL" r:id="rId43" sheetId="42"/>
+    <sheet name="02Nov2020 17.06.08(IST)-LOCAL" r:id="rId44" sheetId="43"/>
+    <sheet name="23Nov2020 18.17.47(IST)-LOCAL" r:id="rId45" sheetId="44"/>
+    <sheet name="23Nov2020 18.20.31(IST)-LOCAL" r:id="rId46" sheetId="45"/>
+    <sheet name="23Nov2020 18.25.21(IST)-LOCAL" r:id="rId47" sheetId="46"/>
+    <sheet name="23Nov2020 19.53.52(IST)-LOCAL" r:id="rId48" sheetId="47"/>
+    <sheet name="23Nov2020 19.56.50(IST)-LOCAL" r:id="rId49" sheetId="48"/>
+    <sheet name="23Nov2020 20.48.24(IST)-LOCAL" r:id="rId50" sheetId="49"/>
+    <sheet name="23Nov2020 20.56.20(IST)-LOCAL" r:id="rId51" sheetId="50"/>
+    <sheet name="23Nov2020 21.03.00(IST)-LOCAL" r:id="rId52" sheetId="51"/>
+    <sheet name="23Nov2020 21.06.24(IST)-LOCAL" r:id="rId53" sheetId="52"/>
+    <sheet name="23Nov2020 21.11.28(IST)-LOCAL" r:id="rId54" sheetId="53"/>
+    <sheet name="25Nov2020 19.14.27(IST)-LOCAL" r:id="rId55" sheetId="54"/>
+    <sheet name="25Nov2020 19.21.53(IST)-LOCAL" r:id="rId56" sheetId="55"/>
+    <sheet name="25Nov2020 19.24.25(IST)-LOCAL" r:id="rId57" sheetId="56"/>
+    <sheet name="25Nov2020 19.29.03(IST)-LOCAL" r:id="rId58" sheetId="57"/>
+    <sheet name="25Nov2020 19.34.26(IST)-LOCAL" r:id="rId59" sheetId="58"/>
+    <sheet name="25Nov2020 19.44.08(IST)-LOCAL" r:id="rId60" sheetId="59"/>
+    <sheet name="25Nov2020 19.49.35(IST)-LOCAL" r:id="rId61" sheetId="60"/>
+    <sheet name="25Nov2020 19.56.42(IST)-LOCAL" r:id="rId62" sheetId="61"/>
+    <sheet name="25Nov2020 20.09.22(IST)-LOCAL" r:id="rId63" sheetId="62"/>
+    <sheet name="25Nov2020 20.13.55(IST)-LOCAL" r:id="rId64" sheetId="63"/>
+    <sheet name="25Nov2020 20.14.21(IST)-LOCAL" r:id="rId65" sheetId="64"/>
+    <sheet name="25Nov2020 20.38.01(IST)-LOCAL" r:id="rId66" sheetId="65"/>
+    <sheet name="25Nov2020 20.41.25(IST)-LOCAL" r:id="rId67" sheetId="66"/>
+    <sheet name="30Nov2020 16.33.07(IST)-LOCAL" r:id="rId68" sheetId="67"/>
+    <sheet name="08Dec2020 17.47.22(IST)-LOCAL" r:id="rId69" sheetId="68"/>
+    <sheet name="08Dec2020 17.58.04(IST)-LOCAL" r:id="rId70" sheetId="69"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1427" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1901" uniqueCount="380">
   <si>
     <t>DataType</t>
   </si>
@@ -1072,6 +1124,102 @@
   </si>
   <si>
     <t>https://mcpperf.wsgc.com/</t>
+  </si>
+  <si>
+    <t>Merch List &gt; WE &gt; Furniture&gt;806 - WE CASUAL SEATING &gt; WE Furniture Fall 2020 - Page 1</t>
+  </si>
+  <si>
+    <t>Merch List &gt; WE &gt; Furniture&gt;806 - WE CASUAL SEATING &gt; WE Furniture Fall 2020 - Page 2</t>
+  </si>
+  <si>
+    <t>Merch List &gt; WE &gt; Furniture&gt;806 - WE CASUAL SEATING &gt; WE Furniture Fall 2020 - Page 3</t>
+  </si>
+  <si>
+    <t>Merch List &gt; WE &gt; Furniture&gt;806 - WE CASUAL SEATING &gt; WE Furniture Fall 2020 - Page 4</t>
+  </si>
+  <si>
+    <t>Merch List &gt; WE &gt; Furniture&gt;806 - WE CASUAL SEATING &gt; WE Furniture Fall 2020 - Page 5</t>
+  </si>
+  <si>
+    <t>After Update &gt; Page 1</t>
+  </si>
+  <si>
+    <t>After Update &gt; Page 2</t>
+  </si>
+  <si>
+    <t>After Update &gt; Page 3</t>
+  </si>
+  <si>
+    <t>After Update &gt; Page 4</t>
+  </si>
+  <si>
+    <t>After Update &gt; Page 5</t>
+  </si>
+  <si>
+    <t>VLL &gt; WE &gt; Furniture&gt;806 - WE CASUAL SEATING &gt; WE Furniture Fall 2020 - Page 1</t>
+  </si>
+  <si>
+    <t>VLL &gt; WE &gt; Furniture&gt;806 - WE CASUAL SEATING &gt; WE Furniture Fall 2020 - Page 2</t>
+  </si>
+  <si>
+    <t>VLL &gt; WE &gt; Furniture&gt;806 - WE CASUAL SEATING &gt; WE Furniture Fall 2020 - Page 3</t>
+  </si>
+  <si>
+    <t>VLL &gt; WE &gt; Furniture&gt;806 - WE CASUAL SEATING &gt; WE Furniture Fall 2020 - Page 4</t>
+  </si>
+  <si>
+    <t>VLL &gt; WE &gt; Furniture&gt;806 - WE CASUAL SEATING &gt; WE Furniture Fall 2020 - Page 5</t>
+  </si>
+  <si>
+    <t>Merch List &gt; WE &gt; Lighting&gt;805 - WE LIGHTING &gt; WE Lighting Fall 2020 - Page 1</t>
+  </si>
+  <si>
+    <t>http://10.180.6.163:443/</t>
+  </si>
+  <si>
+    <t>Mass Edit Merch List &gt; WE &gt; Furniture&gt;806 - WE CASUAL SEATING &gt; WE Furniture Fall 2020</t>
+  </si>
+  <si>
+    <t>Mass Edit Merch List &gt; WE &gt; Lighting&gt;805 - WE LIGHTING &gt; WE Lighting Fall 2020</t>
+  </si>
+  <si>
+    <t>Sub Class Description Mass Edit Merch List &gt; WE &gt; Lighting&gt;805 - WE LIGHTING &gt; WE Lighting Fall 2020</t>
+  </si>
+  <si>
+    <t>Item Type Mass Edit Merch List &gt; WE &gt; Lighting&gt;805 - WE LIGHTING &gt; WE Lighting Fall 2020</t>
+  </si>
+  <si>
+    <t>Fabric Mill Name/Number Mass Edit Merch List &gt; WE &gt; Lighting&gt;805 - WE LIGHTING &gt; WE Lighting Fall 2020</t>
+  </si>
+  <si>
+    <t>Fair Trade Flag Mass Edit Merch List &gt; WE &gt; Lighting&gt;805 - WE LIGHTING &gt; WE Lighting Fall 2020</t>
+  </si>
+  <si>
+    <t>Sub Class Description &gt; Mass Edit &gt; Merch List &gt; WE &gt; Furniture&gt;806 - WE CASUAL SEATING &gt; WE Furniture Fall 2020</t>
+  </si>
+  <si>
+    <t>Item Type &gt; Mass Edit &gt; Merch List &gt; WE &gt; Furniture&gt;806 - WE CASUAL SEATING &gt; WE Furniture Fall 2020</t>
+  </si>
+  <si>
+    <t>Fabric Mill Name/Number &gt; Mass Edit &gt; Merch List &gt; WE &gt; Furniture&gt;806 - WE CASUAL SEATING &gt; WE Furniture Fall 2020</t>
+  </si>
+  <si>
+    <t>Fair Trade Flag &gt; Mass Edit &gt;Merch List &gt; WE &gt; Furniture&gt;806 - WE CASUAL SEATING &gt; WE Furniture Fall 2020</t>
+  </si>
+  <si>
+    <t>Sub Class Description &gt; Mass Edit &gt; Merch List &gt; WE &gt; Lighting&gt;805 - WE LIGHTING &gt; WE Lighting Fall 2020</t>
+  </si>
+  <si>
+    <t>Item Type &gt; Mass Edit &gt; Merch List &gt; WE &gt; Lighting&gt;805 - WE LIGHTING &gt; WE Lighting Fall 2020</t>
+  </si>
+  <si>
+    <t>Fabric Mill Name/Number &gt; Mass Edit &gt; Merch List &gt; WE &gt; Lighting&gt;805 - WE LIGHTING &gt; WE Lighting Fall 2020</t>
+  </si>
+  <si>
+    <t>Fair Trade Flag &gt; Mass Edit &gt;Merch List &gt; WE &gt; Lighting&gt;805 - WE LIGHTING &gt; WE Lighting Fall 2020</t>
+  </si>
+  <si>
+    <t>Create Placeholder &gt; WE Lighting Fall 2020</t>
   </si>
 </sst>
 </file>
@@ -8665,6 +8813,218 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1742.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>43244.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1742.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>722.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="n">
+        <v>25090.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>349</v>
+      </c>
+      <c r="B6" t="n">
+        <v>25090.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>15362.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>350</v>
+      </c>
+      <c r="B7" t="n">
+        <v>25090.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>12199.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>351</v>
+      </c>
+      <c r="B8" t="n">
+        <v>25090.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>20956.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>352</v>
+      </c>
+      <c r="B9" t="n">
+        <v>25090.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>16675.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>340</v>
+      </c>
+      <c r="B10" t="n">
+        <v>25090.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>499.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>348</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1644.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>25578.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>349</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1644.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>19875.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>350</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1644.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>18998.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>351</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1644.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>21342.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>352</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1644.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>26158.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1521.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>32910.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr>
@@ -8837,6 +9197,1638 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2124.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>19459.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2124.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>508.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1168.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>51367.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>353</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1168.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>29045.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>349</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1168.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>27626.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1168.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>31076.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>350</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1168.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>47762.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>355</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1168.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>27194.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>351</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1168.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>29180.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>356</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1168.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>28425.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>352</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1168.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>27246.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>357</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1168.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>28849.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>340</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1168.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>462.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>348</v>
+      </c>
+      <c r="B16" t="n">
+        <v>2853.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>25334.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>353</v>
+      </c>
+      <c r="B17" t="n">
+        <v>2853.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>18652.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>349</v>
+      </c>
+      <c r="B18" t="n">
+        <v>2853.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>21196.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>354</v>
+      </c>
+      <c r="B19" t="n">
+        <v>2853.0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>25015.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>350</v>
+      </c>
+      <c r="B20" t="n">
+        <v>2853.0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>22163.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>355</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2853.0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>27234.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>351</v>
+      </c>
+      <c r="B22" t="n">
+        <v>2853.0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>24940.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>356</v>
+      </c>
+      <c r="B23" t="n">
+        <v>2853.0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>35818.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>352</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2853.0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>29493.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>357</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2853.0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>35740.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1823.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>38953.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1823.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>503.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="n">
+        <v>789.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>41478.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1274.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>18713.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1274.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>425.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="n">
+        <v>822.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>38136.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1217.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9067.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1217.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>543.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1231.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>10296.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1231.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>503.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="n">
+        <v>502.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>28096.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>353</v>
+      </c>
+      <c r="B6" t="n">
+        <v>502.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>36692.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>349</v>
+      </c>
+      <c r="B7" t="n">
+        <v>502.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>26494.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B8" t="n">
+        <v>502.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>35952.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>350</v>
+      </c>
+      <c r="B9" t="n">
+        <v>502.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>26294.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>355</v>
+      </c>
+      <c r="B10" t="n">
+        <v>502.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>34073.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>351</v>
+      </c>
+      <c r="B11" t="n">
+        <v>502.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>25391.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>356</v>
+      </c>
+      <c r="B12" t="n">
+        <v>502.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>30195.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>352</v>
+      </c>
+      <c r="B13" t="n">
+        <v>502.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>25789.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>357</v>
+      </c>
+      <c r="B14" t="n">
+        <v>502.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>30854.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>340</v>
+      </c>
+      <c r="B15" t="n">
+        <v>502.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>448.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>348</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>24648.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>353</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>32669.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>349</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>25456.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>354</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>29103.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>350</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>22407.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>355</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>32177.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>351</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>26854.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>356</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>34193.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>352</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>25606.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>357</v>
+      </c>
+      <c r="B25" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>27264.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>358</v>
+      </c>
+      <c r="B26" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>357.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>359</v>
+      </c>
+      <c r="B27" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>15816.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>360</v>
+      </c>
+      <c r="B28" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>16182.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>361</v>
+      </c>
+      <c r="B29" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>17279.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>362</v>
+      </c>
+      <c r="B30" t="n">
+        <v>1424.0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>20030.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1597.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>15974.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1597.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>543.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>15976.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>353</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>24407.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>349</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>21536.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>31471.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>350</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>22610.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>355</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>32178.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>351</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>25552.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>356</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>20395.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>352</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>14230.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>357</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>39247.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>358</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>17821.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>359</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>15186.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>360</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>15192.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>361</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>16717.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>362</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>16838.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>340</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1356.0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>539.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>348</v>
+      </c>
+      <c r="B21" t="n">
+        <v>2345.0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>15787.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>353</v>
+      </c>
+      <c r="B22" t="n">
+        <v>2345.0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>25454.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>349</v>
+      </c>
+      <c r="B23" t="n">
+        <v>2345.0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>16195.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>354</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2345.0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>26098.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>350</v>
+      </c>
+      <c r="B25" t="n">
+        <v>2345.0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>14088.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>355</v>
+      </c>
+      <c r="B26" t="n">
+        <v>2345.0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>28758.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>351</v>
+      </c>
+      <c r="B27" t="n">
+        <v>2345.0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>19051.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>356</v>
+      </c>
+      <c r="B28" t="n">
+        <v>2345.0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>31775.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>352</v>
+      </c>
+      <c r="B29" t="n">
+        <v>2345.0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>22120.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>357</v>
+      </c>
+      <c r="B30" t="n">
+        <v>2345.0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>28290.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>358</v>
+      </c>
+      <c r="B31" t="n">
+        <v>2345.0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>18313.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>359</v>
+      </c>
+      <c r="B32" t="n">
+        <v>2345.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>16791.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>360</v>
+      </c>
+      <c r="B33" t="n">
+        <v>2345.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>17872.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>361</v>
+      </c>
+      <c r="B34" t="n">
+        <v>2345.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>13766.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>362</v>
+      </c>
+      <c r="B35" t="n">
+        <v>2345.0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>15368.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2022.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>22325.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2022.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>530.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2739.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>19305.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2739.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>703.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1293.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>47932.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>353</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1293.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>44211.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>349</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1293.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>42166.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1293.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>38712.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>350</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1293.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>35343.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>355</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1293.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>30343.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>351</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1293.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>23403.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>356</v>
+      </c>
+      <c r="B12" t="n">
+        <v>1293.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>30796.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>352</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1293.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>20304.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>357</v>
+      </c>
+      <c r="B14" t="n">
+        <v>1293.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>30063.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>358</v>
+      </c>
+      <c r="B15" t="n">
+        <v>1293.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>32209.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>359</v>
+      </c>
+      <c r="B16" t="n">
+        <v>1293.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>25181.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>360</v>
+      </c>
+      <c r="B17" t="n">
+        <v>1293.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>24887.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>361</v>
+      </c>
+      <c r="B18" t="n">
+        <v>1293.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>25605.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>362</v>
+      </c>
+      <c r="B19" t="n">
+        <v>1293.0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>29689.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>340</v>
+      </c>
+      <c r="B20" t="n">
+        <v>1293.0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>641.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>348</v>
+      </c>
+      <c r="B21" t="n">
+        <v>1859.0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>28408.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>353</v>
+      </c>
+      <c r="B22" t="n">
+        <v>1859.0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>28512.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>349</v>
+      </c>
+      <c r="B23" t="n">
+        <v>1859.0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>19777.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>354</v>
+      </c>
+      <c r="B24" t="n">
+        <v>1859.0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>26258.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1601.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>16007.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1601.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>594.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="n">
+        <v>923.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>35151.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1520.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11316.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1520.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>594.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1184.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>32428.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr>
@@ -9025,6 +11017,824 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1397.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>12722.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1397.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>599.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="n">
+        <v>676.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>25771.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>353</v>
+      </c>
+      <c r="B6" t="n">
+        <v>676.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>33820.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>349</v>
+      </c>
+      <c r="B7" t="n">
+        <v>676.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>25613.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1169.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>12298.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1169.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>609.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2563.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>34001.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2146.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>18559.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2146.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>498.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>43941.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>353</v>
+      </c>
+      <c r="B6" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>43036.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>349</v>
+      </c>
+      <c r="B7" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>26262.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>354</v>
+      </c>
+      <c r="B8" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>42887.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>350</v>
+      </c>
+      <c r="B9" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>27337.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>355</v>
+      </c>
+      <c r="B10" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>45007.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>351</v>
+      </c>
+      <c r="B11" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>28089.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>356</v>
+      </c>
+      <c r="B12" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>34926.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>352</v>
+      </c>
+      <c r="B13" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>41216.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>357</v>
+      </c>
+      <c r="B14" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>52290.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>358</v>
+      </c>
+      <c r="B15" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>29373.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>359</v>
+      </c>
+      <c r="B16" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>27747.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>360</v>
+      </c>
+      <c r="B17" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>40703.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>361</v>
+      </c>
+      <c r="B18" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>26353.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>362</v>
+      </c>
+      <c r="B19" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>28209.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>340</v>
+      </c>
+      <c r="B20" t="n">
+        <v>902.0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>540.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>348</v>
+      </c>
+      <c r="B21" t="n">
+        <v>939.0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>30696.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>353</v>
+      </c>
+      <c r="B22" t="n">
+        <v>939.0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>33888.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>349</v>
+      </c>
+      <c r="B23" t="n">
+        <v>939.0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>36994.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>354</v>
+      </c>
+      <c r="B24" t="n">
+        <v>939.0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>38617.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>350</v>
+      </c>
+      <c r="B25" t="n">
+        <v>939.0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>29294.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>355</v>
+      </c>
+      <c r="B26" t="n">
+        <v>939.0</v>
+      </c>
+      <c r="C26" t="n">
+        <v>44027.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>351</v>
+      </c>
+      <c r="B27" t="n">
+        <v>939.0</v>
+      </c>
+      <c r="C27" t="n">
+        <v>30170.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>356</v>
+      </c>
+      <c r="B28" t="n">
+        <v>939.0</v>
+      </c>
+      <c r="C28" t="n">
+        <v>38201.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>352</v>
+      </c>
+      <c r="B29" t="n">
+        <v>939.0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>31425.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>357</v>
+      </c>
+      <c r="B30" t="n">
+        <v>939.0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>41241.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>358</v>
+      </c>
+      <c r="B31" t="n">
+        <v>939.0</v>
+      </c>
+      <c r="C31" t="n">
+        <v>29435.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>359</v>
+      </c>
+      <c r="B32" t="n">
+        <v>939.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>56463.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>360</v>
+      </c>
+      <c r="B33" t="n">
+        <v>939.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>61791.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>361</v>
+      </c>
+      <c r="B34" t="n">
+        <v>939.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>56633.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>362</v>
+      </c>
+      <c r="B35" t="n">
+        <v>939.0</v>
+      </c>
+      <c r="C35" t="n">
+        <v>31734.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2090.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>70670.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2090.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>521.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5810.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>39154.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5810.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>476.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4858.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>48716.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3173.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>46229.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3173.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>497.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -9261,6 +12071,527 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1351.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>12564.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1351.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>548.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>363</v>
+      </c>
+      <c r="B5" t="n">
+        <v>870.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6959.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1181.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11654.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1181.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>461.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>363</v>
+      </c>
+      <c r="B5" t="n">
+        <v>769.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>6994.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>8588.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>25194.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>8588.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>450.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>363</v>
+      </c>
+      <c r="B5" t="n">
+        <v>13096.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>7845.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1560.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11458.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1560.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>552.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>363</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1185.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>9005.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1554.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>15964.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1554.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>595.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1289.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11233.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1289.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>521.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2101.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>14513.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2018.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>24143.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2018.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>703.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2208.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>31925.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2208.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>478.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <sheetPr/>
@@ -9462,6 +12793,626 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
   <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5546.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>74850.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>5546.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>506.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>365</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1109.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>69111.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3179.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>43050.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3179.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>479.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2311.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>16512.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2311.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>757.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>366</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1686.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>16761.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>3403.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>61378.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3403.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>475.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>366</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2071.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>13284.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1086.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9212.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1086.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>481.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>367</v>
+      </c>
+      <c r="B5" t="n">
+        <v>578.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>67481.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1014.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8796.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1014.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>450.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>951.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>8896.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>951.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>522.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>367</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2740.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>67812.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1090.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>12423.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1090.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>519.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>367</v>
+      </c>
+      <c r="B5" t="n">
+        <v>625.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>67066.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1200.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9894.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1200.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>498.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>367</v>
+      </c>
+      <c r="B5" t="n">
+        <v>738.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>67056.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>368</v>
+      </c>
+      <c r="B6" t="n">
+        <v>738.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>67637.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B7" t="n">
+        <v>738.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>66858.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>370</v>
+      </c>
+      <c r="B8" t="n">
+        <v>738.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>67447.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1054.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9305.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1054.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>455.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -11455,6 +15406,637 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>922.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>18449.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>922.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>488.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>367</v>
+      </c>
+      <c r="B5" t="n">
+        <v>661.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>28590.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>368</v>
+      </c>
+      <c r="B6" t="n">
+        <v>661.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>27094.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B7" t="n">
+        <v>661.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>20677.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>370</v>
+      </c>
+      <c r="B8" t="n">
+        <v>661.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>20043.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>971.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>9539.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>971.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>447.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>367</v>
+      </c>
+      <c r="B5" t="n">
+        <v>567.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>18014.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>368</v>
+      </c>
+      <c r="B6" t="n">
+        <v>567.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>15786.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B7" t="n">
+        <v>567.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>17150.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>370</v>
+      </c>
+      <c r="B8" t="n">
+        <v>567.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>15747.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1346.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>11700.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1346.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>516.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6965.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>45523.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1298.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>19886.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1298.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>467.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>371</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1069.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>68465.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>372</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1069.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>71615.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>373</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1069.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>68641.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>374</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1069.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>68271.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1713.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>14309.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1713.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>543.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1098.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>37717.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>376</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1098.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>32764.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>377</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1098.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>26107.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>378</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1098.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>24078.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>339</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1512.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>10982.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>340</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1512.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>495.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>375</v>
+      </c>
+      <c r="B5" t="n">
+        <v>967.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>36896.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B3" t="n">
+        <v>963.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>10046.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <dimension ref="A1:D15"/>

</xml_diff>